<commit_message>
Agrego link de casos de prueba a matriz_pruebas
</commit_message>
<xml_diff>
--- a/casos_de_prueba/matriz_pruebas.xlsx
+++ b/casos_de_prueba/matriz_pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayra\Desktop\ProyectoFinal-ChazarretaMayra\casos_de_prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEBEBDB-81D3-432D-9EFA-EAA438625C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC72D0C-A3CA-4118-9EB1-1FBF636E525F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1NdRKcFUBwytjB3xhmOh6yPCHCwd7VqLOaN6Vfuk-G4w/edit?gid=276038343#gid=276038343</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -65,8 +69,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,13 +356,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="40.5703125" customWidth="1"/>
     <col min="2" max="2" width="34.85546875" customWidth="1"/>
     <col min="3" max="3" width="28.7109375" customWidth="1"/>
     <col min="4" max="4" width="33.42578125" customWidth="1"/>
@@ -367,7 +372,11 @@
     <col min="10" max="10" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>